<commit_message>
Improved pin use and standardized connectors
</commit_message>
<xml_diff>
--- a/handkontroll_ali_BOM.xlsx
+++ b/handkontroll_ali_BOM.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\GitHub\handkontroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C464507B-2131-4A11-8BC2-81F569FF4941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76741BC-95C1-426A-819A-2D2901C9A2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15810" windowHeight="9945" xr2:uid="{86050BAC-365A-4F4D-8610-790F95CF251C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{86050BAC-365A-4F4D-8610-790F95CF251C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="IOs 1.6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="95">
   <si>
     <t>Beskrivelse/navn på varen</t>
   </si>
@@ -201,6 +202,126 @@
   </si>
   <si>
     <t>Total kostnad per handkontroll</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Special function</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Button1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Led1</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>Button2</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Led2</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>Button3</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>Led3</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>Button4</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>Led4</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>PWM_Motor</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>Direction_Motor</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>Run_Motor</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>SDA_I2C</t>
+  </si>
+  <si>
+    <t>LCD_Screen</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>SCL_I2C</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>AnalogRead</t>
+  </si>
+  <si>
+    <t>I2C</t>
   </si>
 </sst>
 </file>
@@ -292,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -416,6 +537,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -423,7 +559,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -465,21 +601,6 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -496,6 +617,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -517,9 +659,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -557,7 +699,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -663,7 +805,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -805,7 +947,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -815,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2001B205-E3DD-4EA4-B17F-435037E0B3D6}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -1280,11 +1422,11 @@
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="4" t="s">
         <v>51</v>
       </c>
@@ -1311,11 +1453,11 @@
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="6">
         <v>25</v>
       </c>
@@ -1332,7 +1474,7 @@
         <f>G2/E2/1.25</f>
         <v>3.5520000000000005</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="26">
         <f>H2*I2</f>
         <v>3.5520000000000005</v>
       </c>
@@ -1345,32 +1487,32 @@
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="6">
         <v>25</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="22">
         <v>179</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="25">
         <v>2485</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="21">
         <f>G3/100/1.25</f>
         <v>19.880000000000003</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="26">
         <f t="shared" ref="J3:J19" si="0">H3*I3</f>
         <v>19.880000000000003</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="24" t="s">
         <v>8</v>
       </c>
       <c r="O3" s="1"/>
@@ -1379,32 +1521,32 @@
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="6">
         <v>25</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="22">
         <v>179</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="25">
         <v>2485</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="21">
         <f>G4/100/1.25</f>
         <v>19.880000000000003</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="26">
         <f t="shared" si="0"/>
         <v>19.880000000000003</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="24" t="s">
         <v>8</v>
       </c>
       <c r="O4" s="1"/>
@@ -1413,32 +1555,32 @@
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="6">
         <v>25</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="22">
         <v>179</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="25">
         <v>2485</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="21">
         <f>G5/100/1.25</f>
         <v>19.880000000000003</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="26">
         <f t="shared" si="0"/>
         <v>19.880000000000003</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="24" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="1"/>
@@ -1447,32 +1589,32 @@
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="6">
         <v>25</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="22">
         <v>179</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="25">
         <v>2485</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="21">
         <f>G6/100/1.25</f>
         <v>19.880000000000003</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="26">
         <f t="shared" si="0"/>
         <v>19.880000000000003</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="24" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="1"/>
@@ -1481,11 +1623,11 @@
       <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="6">
         <v>25</v>
       </c>
@@ -1502,7 +1644,7 @@
         <f>G7/E7/1.25</f>
         <v>28.639999999999997</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="26">
         <f t="shared" si="0"/>
         <v>28.639999999999997</v>
       </c>
@@ -1515,11 +1657,11 @@
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="6">
         <v>25</v>
       </c>
@@ -1536,7 +1678,7 @@
         <f>G8/E8/1.25</f>
         <v>16.768000000000001</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="26">
         <f t="shared" si="0"/>
         <v>16.768000000000001</v>
       </c>
@@ -1549,11 +1691,11 @@
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="6">
         <v>25</v>
       </c>
@@ -1570,7 +1712,7 @@
         <f>G9/E9/1.25</f>
         <v>12.16</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="26">
         <f t="shared" si="0"/>
         <v>12.16</v>
       </c>
@@ -1583,32 +1725,32 @@
       <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="6">
         <v>130</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="22">
         <v>70</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="23">
         <v>966</v>
       </c>
       <c r="H10" s="1">
         <v>2</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="21">
         <f>G10/(130*4)/1.25</f>
         <v>1.4861538461538462</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="26">
         <f t="shared" si="0"/>
         <v>2.9723076923076923</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="24" t="s">
         <v>19</v>
       </c>
       <c r="O10" s="1"/>
@@ -1617,32 +1759,32 @@
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="6">
         <v>130</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="22">
         <v>70</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="23">
         <v>966</v>
       </c>
       <c r="H11" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="21">
         <f>G11/(130*4)/1.25</f>
         <v>1.4861538461538462</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="26">
         <f t="shared" si="0"/>
         <v>8.9169230769230765</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="24" t="s">
         <v>19</v>
       </c>
       <c r="O11" s="1"/>
@@ -1651,32 +1793,32 @@
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="6">
         <v>130</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="22">
         <v>70</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="23">
         <v>966</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="21">
         <f>G12/(130*4)/1.25</f>
         <v>1.4861538461538462</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="24" t="s">
         <v>19</v>
       </c>
       <c r="O12" s="1"/>
@@ -1685,11 +1827,11 @@
       <c r="A13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="6">
         <v>25</v>
       </c>
@@ -1703,10 +1845,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="20">
-        <f>G13/E13/1.25</f>
+        <f t="shared" ref="I13:I19" si="1">G13/E13/1.25</f>
         <v>22.496000000000002</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="26">
         <f t="shared" si="0"/>
         <v>22.496000000000002</v>
       </c>
@@ -1719,11 +1861,11 @@
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="6">
         <v>40</v>
       </c>
@@ -1737,10 +1879,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="20">
-        <f>G14/E14/1.25</f>
+        <f t="shared" si="1"/>
         <v>1.72</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="26">
         <f t="shared" si="0"/>
         <v>1.72</v>
       </c>
@@ -1753,11 +1895,11 @@
       <c r="A15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="6">
         <v>30</v>
       </c>
@@ -1771,10 +1913,10 @@
         <v>1</v>
       </c>
       <c r="I15" s="20">
-        <f>G15/E15/1.25</f>
+        <f t="shared" si="1"/>
         <v>1.44</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="26">
         <f t="shared" si="0"/>
         <v>1.44</v>
       </c>
@@ -1787,11 +1929,11 @@
       <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="6">
         <v>100</v>
       </c>
@@ -1805,10 +1947,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="20">
-        <f>G16/E16/1.25</f>
+        <f t="shared" si="1"/>
         <v>0.91199999999999992</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="26">
         <f t="shared" si="0"/>
         <v>0.91199999999999992</v>
       </c>
@@ -1821,11 +1963,11 @@
       <c r="A17" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="6">
         <v>100</v>
       </c>
@@ -1839,10 +1981,10 @@
         <v>4</v>
       </c>
       <c r="I17" s="20">
-        <f>G17/E17/1.25</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="26">
         <f t="shared" si="0"/>
         <v>2.08</v>
       </c>
@@ -1855,11 +1997,11 @@
       <c r="A18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="6">
         <v>60</v>
       </c>
@@ -1873,10 +2015,10 @@
         <v>2</v>
       </c>
       <c r="I18" s="20">
-        <f>G18/E18/1.25</f>
+        <f t="shared" si="1"/>
         <v>0.85333333333333328</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="26">
         <f t="shared" si="0"/>
         <v>1.7066666666666666</v>
       </c>
@@ -1889,11 +2031,11 @@
       <c r="A19" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="6">
         <v>40</v>
       </c>
@@ -1907,10 +2049,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="20">
-        <f>G19/E19/1.25</f>
+        <f t="shared" si="1"/>
         <v>2.08</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="26">
         <f t="shared" si="0"/>
         <v>2.08</v>
       </c>
@@ -1921,9 +2063,9 @@
     </row>
     <row r="20" spans="1:15" ht="33.75" customHeight="1" thickBot="1">
       <c r="A20" s="11"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="8" t="s">
         <v>1</v>
       </c>
@@ -1939,7 +2081,7 @@
       <c r="I20" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="26">
         <f>SUM(J2:J19)</f>
         <v>184.96389743589748</v>
       </c>
@@ -1948,9 +2090,9 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="I21" s="13"/>
       <c r="J21" s="1"/>
       <c r="K21" s="16"/>
@@ -1997,6 +2139,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B20:D20"/>
@@ -2013,18 +2160,316 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7F7658-8CBC-4C8F-A4AB-C301AED2C5F4}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A2" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="32"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A3" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="32"/>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A5" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A6" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A7" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="32"/>
+    </row>
+    <row r="8" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A8" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A9" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A10" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A11" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A12" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="32"/>
+    </row>
+    <row r="13" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A13" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A14" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A15" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" thickBot="1">
+      <c r="A16" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Kommentar xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Tekst xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Forslag_x0020_karakter_x0020_Petter xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <TaxCatchAll xmlns="02888fe1-7cec-4f41-84cc-8be3d6639e71" xsi:nil="true"/>
+    <Karakter_x0020_fremf_x00f8_ring xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Dato xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Karakter_x0020_skriftelig xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <LMS_Mappings xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Teachers xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Student_Groups xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Math_Settings xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Students xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Has_Teacher_Only_SectionGroup xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <AppVersion xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Invited_Teachers xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Templates xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <TeamsChannelId xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <NotebookType xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Distribution_Groups xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Invited_Students xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <FolderType xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <CultureName xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
+    <Owner xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010093848318F01FFC4A96381909532B2949" ma:contentTypeVersion="52" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="38567b0408029abaf94b441676f62e37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02888fe1-7cec-4f41-84cc-8be3d6639e71" xmlns:ns3="0431e43e-dcd7-4536-abea-5fb81c96588e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad2494e5702b537b6c8a56524b6303f7" ns2:_="" ns3:_="">
     <xsd:import namespace="02888fe1-7cec-4f41-84cc-8be3d6639e71"/>
@@ -2514,78 +2959,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Kommentar xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Tekst xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Forslag_x0020_karakter_x0020_Petter xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <TaxCatchAll xmlns="02888fe1-7cec-4f41-84cc-8be3d6639e71" xsi:nil="true"/>
-    <Karakter_x0020_fremf_x00f8_ring xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Dato xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Karakter_x0020_skriftelig xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <LMS_Mappings xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Teachers xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Student_Groups xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Math_Settings xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Students xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Has_Teacher_Only_SectionGroup xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <AppVersion xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Invited_Teachers xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Templates xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <TeamsChannelId xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <NotebookType xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Distribution_Groups xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Invited_Students xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <FolderType xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <CultureName xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e" xsi:nil="true"/>
-    <Owner xmlns="0431e43e-dcd7-4536-abea-5fb81c96588e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE6B01ED-7DB8-4537-8700-D7A7587F6E92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14690D5F-FC5F-471C-82CB-33F4306CFCBA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0431e43e-dcd7-4536-abea-5fb81c96588e"/>
+    <ds:schemaRef ds:uri="02888fe1-7cec-4f41-84cc-8be3d6639e71"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E60D9E-9A24-44E9-AE4A-86A128DDCAA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2602,23 +2995,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14690D5F-FC5F-471C-82CB-33F4306CFCBA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0431e43e-dcd7-4536-abea-5fb81c96588e"/>
-    <ds:schemaRef ds:uri="02888fe1-7cec-4f41-84cc-8be3d6639e71"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE6B01ED-7DB8-4537-8700-D7A7587F6E92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>